<commit_message>
Made mods to this week's TPS
</commit_message>
<xml_diff>
--- a/Docs/Reports/TPS/TPS Report Main Project [11] - Sept 21 - Sept 27.xlsx
+++ b/Docs/Reports/TPS/TPS Report Main Project [11] - Sept 21 - Sept 27.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odi-setup\Desktop\Git\Team3.14\Docs\Reports\TPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgf0712\Desktop\Git\Team3.14\Docs\Reports\TPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Set Date:</t>
   </si>
@@ -81,10 +81,19 @@
     <t>3 hour</t>
   </si>
   <si>
-    <t>4 Hours</t>
-  </si>
-  <si>
-    <t>1.5 Hours</t>
+    <t>7 Hours</t>
+  </si>
+  <si>
+    <t>3 Hours</t>
+  </si>
+  <si>
+    <t>Create Ruby Version of Site</t>
+  </si>
+  <si>
+    <t>45 Hours</t>
+  </si>
+  <si>
+    <t>12 Hours</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="A1:XFD1048576"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -550,13 +559,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -570,7 +579,7 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -579,6 +588,26 @@
         <v>0.1</v>
       </c>
       <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F14" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>